<commit_message>
Updating the Dataset and prediction code
</commit_message>
<xml_diff>
--- a/MyProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
+++ b/MyProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42508FC0-5C74-4D11-9D02-AF76D47A5226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D41F6C-AE66-44FA-8E38-7F378BC8D028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="79">
   <si>
     <t>Experiment Number</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>InputDimensions</t>
-  </si>
-  <si>
-    <t>Experiment Github URL</t>
   </si>
   <si>
     <t>64x64</t>
@@ -123,22 +120,6 @@
 macro corelation(82-64%) micro corelation(99-92%)</t>
   </si>
   <si>
-    <t>valid output but macro corelation are higher
-macro corelation(89-72%) micro corelation(99-93%)</t>
-  </si>
-  <si>
-    <t>valid output but macro corelation are higher
-macro corelation(97-90%) micro corelation(100-97%)</t>
-  </si>
-  <si>
-    <t>valid, circle-rectangle macro correlation is high
-macro corelation(88-18.8%) micro corelation(96-79%)</t>
-  </si>
-  <si>
-    <t>valid, circle-rectangle macro correlation is high
-macro corelation(80-40%) micro corelation(96-85%)</t>
-  </si>
-  <si>
     <t>output-13</t>
   </si>
   <si>
@@ -285,14 +266,68 @@
   </si>
   <si>
     <t>Result(micro and macro corelation where the percentages refer to the maximun and minimum values from all the shapes)</t>
+  </si>
+  <si>
+    <t>Experiment output image(Github URL- https://github.com/GurunagSai/neocortexapi-classification/tree/pre-main/MyProject/Dataset%20Reports/Dataset-GurunagSai)</t>
+  </si>
+  <si>
+    <t>output-35</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>BEST OUTPUT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,
+macro corelation(46-4%) micro corelation(87-47%)</t>
+    </r>
+  </si>
+  <si>
+    <t>circle-rectangle macro correlation is high
+macro corelation(80-40%) micro corelation(96-85%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> circle-rectangle macro correlation is high
+macro corelation(88-18.8%) micro corelation(96-79%)</t>
+  </si>
+  <si>
+    <t>macro corelation are higher
+macro corelation(97-90%) micro corelation(100-97%)</t>
+  </si>
+  <si>
+    <t>macro corelation are higher
+macro corelation(89-72%) micro corelation(99-93%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -391,7 +426,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -672,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +724,7 @@
     <col min="5" max="5" width="28.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="65.28515625" customWidth="1"/>
     <col min="9" max="9" width="71.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -703,13 +740,13 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="11" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="4" t="s">
         <v>4</v>
@@ -749,16 +786,16 @@
         <v>-1</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -778,16 +815,16 @@
         <v>-1</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -807,16 +844,16 @@
         <v>-1</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -836,16 +873,16 @@
         <v>-1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -865,16 +902,16 @@
         <v>-1</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -894,16 +931,16 @@
         <v>-1</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -923,16 +960,16 @@
         <v>-1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -952,16 +989,16 @@
         <v>-1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -981,16 +1018,16 @@
         <v>-1</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,16 +1047,16 @@
         <v>-1</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1039,16 +1076,16 @@
         <v>-1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1068,16 +1105,16 @@
         <v>-1</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1097,16 +1134,16 @@
         <v>-1</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1126,16 +1163,16 @@
         <v>-1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1155,16 +1192,16 @@
         <v>-1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1184,16 +1221,16 @@
         <v>-1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1213,16 +1250,16 @@
         <v>-1</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H19" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1242,16 +1279,16 @@
         <v>-1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1271,16 +1308,16 @@
         <v>-1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1300,16 +1337,16 @@
         <v>-1</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1329,16 +1366,16 @@
         <v>-1</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H23" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1358,16 +1395,16 @@
         <v>-1</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H24" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1387,16 +1424,16 @@
         <v>-1</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1416,16 +1453,16 @@
         <v>-1</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1445,16 +1482,16 @@
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1474,16 +1511,16 @@
         <v>20</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1503,16 +1540,16 @@
         <v>50</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1532,16 +1569,16 @@
         <v>100</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H30" s="5" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1561,16 +1598,16 @@
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H31" s="5" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1590,16 +1627,16 @@
         <v>50</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H32" s="5" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1619,16 +1656,16 @@
         <v>100</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H33" s="5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1648,16 +1685,16 @@
         <v>100</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1677,16 +1714,16 @@
         <v>-1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1706,16 +1743,45 @@
         <v>-1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H36" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" s="2">
+        <v>30</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E37" s="2">
+        <v>-1</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update output folder URL in excel report
</commit_message>
<xml_diff>
--- a/MyProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
+++ b/MyProject/Dataset Reports/Dataset-GurunagSai/Experiment Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\ExperimentReport\DataSet-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gurunag Sai\source\repos\neocortexapi-classification\MyProject\Dataset Reports\Dataset-GurunagSai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D41F6C-AE66-44FA-8E38-7F378BC8D028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD0050B3-1162-4D86-8819-6A504B90A5DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="2565" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -266,9 +266,6 @@
   </si>
   <si>
     <t>Result(micro and macro corelation where the percentages refer to the maximun and minimum values from all the shapes)</t>
-  </si>
-  <si>
-    <t>Experiment output image(Github URL- https://github.com/GurunagSai/neocortexapi-classification/tree/pre-main/MyProject/Dataset%20Reports/Dataset-GurunagSai)</t>
   </si>
   <si>
     <t>output-35</t>
@@ -312,6 +309,9 @@
   <si>
     <t>macro corelation are higher
 macro corelation(89-72%) micro corelation(99-93%)</t>
+  </si>
+  <si>
+    <t>Experiment output (Github URL-https://github.com/GurunagSai/neocortexapi-classification/tree/main/MyProject/Dataset%20Reports/Dataset-GurunagSai/OutputFolder)</t>
   </si>
 </sst>
 </file>
@@ -711,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,7 +724,7 @@
     <col min="5" max="5" width="28.28515625" style="2" customWidth="1"/>
     <col min="6" max="6" width="21.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="65.28515625" customWidth="1"/>
+    <col min="8" max="8" width="70.140625" customWidth="1"/>
     <col min="9" max="9" width="71.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="2"/>
   </cols>
@@ -740,7 +740,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
       <c r="H1" s="11" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I1" s="9" t="s">
         <v>71</v>
@@ -1027,7 +1027,7 @@
         <v>24</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1056,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1085,7 +1085,7 @@
         <v>15</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
         <v>26</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1778,10 +1778,10 @@
         <v>7</v>
       </c>
       <c r="H37" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="I37" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>